<commit_message>
RVA report almost finished
</commit_message>
<xml_diff>
--- a/VI. X-ray line profile analysis/data/béla.xlsx
+++ b/VI. X-ray line profile analysis/data/béla.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RVA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,13 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>d2t</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>lambda</t>
   </si>
@@ -88,12 +77,24 @@
   <si>
     <t>átlag</t>
   </si>
+  <si>
+    <t>2theta</t>
+  </si>
+  <si>
+    <t>d2theta</t>
+  </si>
+  <si>
+    <t>theta_rad</t>
+  </si>
+  <si>
+    <t>d2theta_rad</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,18 +145,8 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="hu-HU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -184,7 +175,6 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -192,33 +182,11 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="hu-HU"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -298,30 +266,21 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000012-0D7D-49CC-9E1E-9FEF0F06D3F8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="683063664"/>
-        <c:axId val="683062416"/>
+        <c:dLbls/>
+        <c:axId val="149870080"/>
+        <c:axId val="149871616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="683063664"/>
+        <c:axId val="149870080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -339,7 +298,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -374,16 +332,15 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="683062416"/>
+        <c:crossAx val="149871616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="683062416"/>
+        <c:axId val="149871616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -401,7 +358,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -436,7 +392,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="683063664"/>
+        <c:crossAx val="149870080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -450,7 +406,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -479,25 +434,15 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="hu-HU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -526,7 +471,6 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -534,43 +478,21 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="hu-HU"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.7692038495188118E-2"/>
-          <c:y val="0.19486111111111112"/>
-          <c:w val="0.88071084864391946"/>
-          <c:h val="0.72088764946048411"/>
+          <c:x val="7.7692038495188132E-2"/>
+          <c:y val="0.19486111111111115"/>
+          <c:w val="0.88071084864391957"/>
+          <c:h val="0.72088764946048423"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -650,30 +572,21 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0C4E-41C7-835F-3D012275D4A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="594670944"/>
-        <c:axId val="594668032"/>
+        <c:dLbls/>
+        <c:axId val="149986304"/>
+        <c:axId val="150000384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="594670944"/>
+        <c:axId val="149986304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -691,7 +604,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -726,16 +638,15 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="594668032"/>
+        <c:crossAx val="150000384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="594668032"/>
+        <c:axId val="150000384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -753,7 +664,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -788,7 +698,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="594670944"/>
+        <c:crossAx val="149986304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -802,7 +712,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -831,25 +740,15 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="hu-HU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -878,7 +777,6 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -886,33 +784,11 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="hu-HU"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -992,30 +868,21 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7FA0-4216-8E32-CCD3C1FCB618}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="594675104"/>
-        <c:axId val="594670944"/>
+        <c:dLbls/>
+        <c:axId val="151073536"/>
+        <c:axId val="151075072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="594675104"/>
+        <c:axId val="151073536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1033,7 +900,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1068,16 +934,15 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="594670944"/>
+        <c:crossAx val="151075072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="594670944"/>
+        <c:axId val="151075072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1095,7 +960,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1130,7 +994,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="594675104"/>
+        <c:crossAx val="151073536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1144,7 +1008,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1173,25 +1036,15 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="hu-HU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1219,7 +1072,17 @@
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
@@ -1229,11 +1092,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.42472900262467195"/>
-          <c:y val="2.7777777777777776E-2"/>
+          <c:x val="0.424729002624672"/>
+          <c:y val="2.777777777777779E-2"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1241,33 +1103,11 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="hu-HU"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1347,30 +1187,21 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-23DD-484D-B603-CB1373C37466}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="594664288"/>
-        <c:axId val="594664704"/>
+        <c:dLbls/>
+        <c:axId val="151111936"/>
+        <c:axId val="150994944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="594664288"/>
+        <c:axId val="151111936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1388,7 +1219,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1423,16 +1253,15 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="594664704"/>
+        <c:crossAx val="150994944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="594664704"/>
+        <c:axId val="150994944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1450,7 +1279,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1485,7 +1313,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="594664288"/>
+        <c:crossAx val="151111936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1499,7 +1327,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1528,7 +1355,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3762,16 +3589,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3792,16 +3619,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3926,7 +3753,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -3961,7 +3788,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -4138,74 +3965,80 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
       <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>0.13426573444442</v>
       </c>
@@ -4221,7 +4054,7 @@
         <v>0.37783760311799242</v>
       </c>
       <c r="E2">
-        <f>(COS(D2)*B2)/$B$10</f>
+        <f t="shared" ref="E2:E7" si="0">(COS(D2)*B2)/$B$10</f>
         <v>1.4137919093548904E-2</v>
       </c>
       <c r="F2">
@@ -4254,7 +4087,7 @@
         <v>0.10175000000000002</v>
       </c>
       <c r="N2">
-        <f t="shared" ref="N2:O7" si="0">$F2^(2)*K2</f>
+        <f t="shared" ref="N2:O7" si="1">$F2^(2)*K2</f>
         <v>3.103920301730136</v>
       </c>
       <c r="O2">
@@ -4266,27 +4099,27 @@
         <v>2.3337746629549896</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>0.23140714788163</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B7" si="1">RADIANS(A3)</f>
+        <f t="shared" ref="B3:B7" si="2">RADIANS(A3)</f>
         <v>4.0388166431838644E-3</v>
       </c>
       <c r="C3">
         <v>50.433</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D7" si="2">RADIANS(C3/2)</f>
+        <f t="shared" ref="D3:D7" si="3">RADIANS(C3/2)</f>
         <v>0.44011095082915008</v>
       </c>
       <c r="E3">
-        <f>(COS(D3)*B3)/$B$10</f>
+        <f t="shared" si="0"/>
         <v>2.3717611223632959E-2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F7" si="3">(2*SIN(D3))/$B$10</f>
+        <f t="shared" ref="F3:F7" si="4">(2*SIN(D3))/$B$10</f>
         <v>5.5308301361979355</v>
       </c>
       <c r="G3" s="1">
@@ -4299,19 +4132,19 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J7" si="4">(G3^(2)*H3^(2)+H3^(2)*I3^(2) + H3^(2) * I3^(2)) / (G3^(2) + H3^(2) + I3^(2))^2</f>
+        <f t="shared" ref="J3:J7" si="5">(G3^(2)*H3^(2)+H3^(2)*I3^(2) + H3^(2) * I3^(2)) / (G3^(2) + H3^(2) + I3^(2))^2</f>
         <v>0</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:M7" si="5">$B$16*(1-$B$11*$J3)</f>
+        <f t="shared" ref="K3:K7" si="6">$B$16*(1-$B$11*$J3)</f>
         <v>0.30525000000000002</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L7" si="6">$B$16*(1-$B$12*$J3)</f>
+        <f t="shared" ref="L3:L7" si="7">$B$16*(1-$B$12*$J3)</f>
         <v>0.30525000000000002</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M7" si="7">$B$16*(1-$B$13*$J3)</f>
+        <f t="shared" ref="M3:M7" si="8">$B$16*(1-$B$13*$J3)</f>
         <v>0.30525000000000002</v>
       </c>
       <c r="N3">
@@ -4319,35 +4152,35 @@
         <v>9.3376225291188284</v>
       </c>
       <c r="O3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.3376225291188284</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P7" si="8">$F3^(2)*M3</f>
+        <f t="shared" ref="P3:P7" si="9">$F3^(2)*M3</f>
         <v>9.3376225291188284</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>0.25945039851653001</v>
       </c>
       <c r="B4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.5282636997248608E-3</v>
       </c>
       <c r="C4">
         <v>74.13</v>
       </c>
       <c r="D4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.64690628725169819</v>
       </c>
       <c r="E4">
-        <f>(COS(D4)*B4)/$B$10</f>
+        <f t="shared" si="0"/>
         <v>2.3454097413699582E-2</v>
       </c>
       <c r="F4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.824492521530316</v>
       </c>
       <c r="G4" s="1">
@@ -4360,55 +4193,55 @@
         <v>2</v>
       </c>
       <c r="J4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="K4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.13532750000000002</v>
       </c>
       <c r="L4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.8172500000000025E-2</v>
       </c>
       <c r="M4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.10175000000000002</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.2851126633846999</v>
       </c>
       <c r="O4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.1737033717802641</v>
       </c>
       <c r="P4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.2294080175824824</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>0.40705561787745997</v>
       </c>
       <c r="B5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.1044607707015685E-3</v>
       </c>
       <c r="C5">
         <v>89.930999999999997</v>
       </c>
       <c r="D5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.78479602480551025</v>
       </c>
       <c r="E5">
-        <f>(COS(D5)*B5)/$B$10</f>
+        <f t="shared" si="0"/>
         <v>3.2627783900012093E-2</v>
       </c>
       <c r="F5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.1740993994877513</v>
       </c>
       <c r="G5" s="1">
@@ -4425,51 +4258,51 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="K5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.25890750000000001</v>
       </c>
       <c r="L5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.24059250000000001</v>
       </c>
       <c r="M5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.24975</v>
       </c>
       <c r="N5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21.790716666814784</v>
       </c>
       <c r="O5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20.249251179130138</v>
       </c>
       <c r="P5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>21.019983922972461</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>0.28457402236714002</v>
       </c>
       <c r="B6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.9667536559505811E-3</v>
       </c>
       <c r="C6">
         <v>95.138999999999996</v>
       </c>
       <c r="D6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.83024439852744258</v>
       </c>
       <c r="E6">
-        <f>(COS(D6)*B6)/$B$10</f>
+        <f t="shared" si="0"/>
         <v>2.1751563013127726E-2</v>
       </c>
       <c r="F6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.5819328535860357</v>
       </c>
       <c r="G6" s="1">
@@ -4482,55 +4315,55 @@
         <v>2</v>
       </c>
       <c r="J6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="K6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.13532750000000002</v>
       </c>
       <c r="L6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.8172500000000025E-2</v>
       </c>
       <c r="M6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.10175000000000002</v>
       </c>
       <c r="N6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.424882924121727</v>
       </c>
       <c r="O6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.2591515482417739</v>
       </c>
       <c r="P6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9.34201723618175</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>0.77615879329966997</v>
       </c>
       <c r="B7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3546526461385345E-2</v>
       </c>
       <c r="C7">
         <v>116.919</v>
       </c>
       <c r="D7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.020310754069625</v>
       </c>
       <c r="E7">
-        <f>(COS(D7)*B7)/$B$10</f>
+        <f t="shared" si="0"/>
         <v>4.5996386465336048E-2</v>
       </c>
       <c r="F7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.064138892675288</v>
       </c>
       <c r="G7" s="1">
@@ -4543,85 +4376,85 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K7">
-        <f t="shared" si="5"/>
-        <v>0.30525000000000002</v>
-      </c>
-      <c r="L7">
         <f t="shared" si="6"/>
         <v>0.30525000000000002</v>
       </c>
-      <c r="M7">
+      <c r="L7">
         <f t="shared" si="7"/>
         <v>0.30525000000000002</v>
       </c>
+      <c r="M7">
+        <f t="shared" si="8"/>
+        <v>0.30525000000000002</v>
+      </c>
       <c r="N7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37.367230470464143</v>
       </c>
       <c r="O7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37.367230470464143</v>
       </c>
       <c r="P7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>37.367230470464143</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B10">
         <v>0.15406</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>1.67</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>2.33</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>0.30759999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15">
         <v>0.3029</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16">
         <f>AVERAGE(B14:B15)</f>

</xml_diff>